<commit_message>
BOM and schematic update
altium
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\max19_000\Documents\GitHub\Power2LabPowerSupply\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sjefen\OneDrive - Danmarks Tekniske Universitet\Skole\Effektelektronik 2\Power2LabPowerSupply\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9465"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9465" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="260">
   <si>
     <t>Circuit Block</t>
   </si>
@@ -581,9 +581,6 @@
     <t>15 V</t>
   </si>
   <si>
-    <t>Enable</t>
-  </si>
-  <si>
     <t>General</t>
   </si>
   <si>
@@ -710,9 +707,6 @@
     <t>10stk</t>
   </si>
   <si>
-    <t>Current sensor</t>
-  </si>
-  <si>
     <t>Diodes INC</t>
   </si>
   <si>
@@ -744,12 +738,78 @@
   </si>
   <si>
     <t>PTV09A-4225F-B102</t>
+  </si>
+  <si>
+    <t>Current sensor IC</t>
+  </si>
+  <si>
+    <t>KOA Speer</t>
+  </si>
+  <si>
+    <t>SR732ATTDR200F</t>
+  </si>
+  <si>
+    <t>660-SR732ATTER200F</t>
+  </si>
+  <si>
+    <t>Roc</t>
+  </si>
+  <si>
+    <t>0.2 R</t>
+  </si>
+  <si>
+    <t>Sense resistor at output</t>
+  </si>
+  <si>
+    <t>Enable,</t>
+  </si>
+  <si>
+    <t>Cout2_1</t>
+  </si>
+  <si>
+    <t>Cout2_2</t>
+  </si>
+  <si>
+    <t>C22</t>
+  </si>
+  <si>
+    <t>C23</t>
+  </si>
+  <si>
+    <t>Rfilt</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>U5A</t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>10 pF</t>
+  </si>
+  <si>
+    <t>4.7 k</t>
+  </si>
+  <si>
+    <t>400 R</t>
+  </si>
+  <si>
+    <t>20 k</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -832,7 +892,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -850,6 +910,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1163,11 +1227,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K98"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G88" sqref="G88"/>
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L96" sqref="L96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1640,172 +1704,172 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>193</v>
+      </c>
+      <c r="B20" t="s">
         <v>194</v>
-      </c>
-      <c r="B20" t="s">
-        <v>195</v>
       </c>
       <c r="C20" t="s">
         <v>9</v>
       </c>
       <c r="D20" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E20" t="s">
         <v>61</v>
       </c>
       <c r="F20" t="s">
+        <v>201</v>
+      </c>
+      <c r="G20" s="4" t="s">
         <v>202</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>203</v>
       </c>
       <c r="H20" t="s">
         <v>10</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J20" s="2"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C21" t="s">
         <v>9</v>
       </c>
       <c r="D21" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E21" t="s">
         <v>61</v>
       </c>
       <c r="F21" t="s">
+        <v>201</v>
+      </c>
+      <c r="G21" s="4" t="s">
         <v>202</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>203</v>
       </c>
       <c r="H21" t="s">
         <v>10</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J21" s="2"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C22" t="s">
         <v>9</v>
       </c>
       <c r="D22" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E22" t="s">
         <v>61</v>
       </c>
       <c r="F22" t="s">
+        <v>201</v>
+      </c>
+      <c r="G22" s="4" t="s">
         <v>202</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>203</v>
       </c>
       <c r="H22" t="s">
         <v>10</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J22" s="2"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C23" t="s">
         <v>9</v>
       </c>
       <c r="D23" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E23" t="s">
         <v>61</v>
       </c>
       <c r="F23" t="s">
+        <v>201</v>
+      </c>
+      <c r="G23" s="4" t="s">
         <v>202</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>203</v>
       </c>
       <c r="H23" t="s">
         <v>10</v>
       </c>
       <c r="I23" s="8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J23" s="2"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C24" t="s">
         <v>9</v>
       </c>
       <c r="D24" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E24" t="s">
         <v>61</v>
       </c>
       <c r="F24" t="s">
+        <v>201</v>
+      </c>
+      <c r="G24" s="4" t="s">
         <v>202</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>203</v>
       </c>
       <c r="H24" t="s">
         <v>10</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J24" s="2"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C25" t="s">
         <v>9</v>
       </c>
       <c r="D25" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E25" t="s">
         <v>61</v>
       </c>
       <c r="F25" t="s">
+        <v>201</v>
+      </c>
+      <c r="G25" s="4" t="s">
         <v>202</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>203</v>
       </c>
       <c r="H25" t="s">
         <v>10</v>
       </c>
       <c r="I25" s="8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J25" s="2"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C26" t="s">
         <v>33</v>
@@ -1823,262 +1887,217 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>206</v>
+        <v>246</v>
       </c>
       <c r="C27" t="s">
-        <v>210</v>
+        <v>9</v>
       </c>
       <c r="D27" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="E27" t="s">
-        <v>218</v>
+        <v>61</v>
       </c>
       <c r="F27" t="s">
-        <v>217</v>
+        <v>201</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>202</v>
       </c>
       <c r="H27" t="s">
         <v>10</v>
       </c>
       <c r="I27" s="8" t="s">
-        <v>219</v>
+        <v>203</v>
       </c>
       <c r="J27" s="2"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>207</v>
+        <v>247</v>
       </c>
       <c r="C28" t="s">
-        <v>210</v>
+        <v>9</v>
       </c>
       <c r="D28" t="s">
-        <v>163</v>
+        <v>200</v>
       </c>
       <c r="E28" t="s">
-        <v>218</v>
+        <v>61</v>
       </c>
       <c r="F28" t="s">
-        <v>217</v>
+        <v>201</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>202</v>
       </c>
       <c r="H28" t="s">
         <v>10</v>
       </c>
       <c r="I28" s="8" t="s">
-        <v>220</v>
+        <v>203</v>
       </c>
       <c r="J28" s="2"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>208</v>
-      </c>
-      <c r="C29" t="s">
-        <v>66</v>
-      </c>
-      <c r="H29" t="s">
-        <v>52</v>
-      </c>
-      <c r="J29" s="5"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>205</v>
+      </c>
+      <c r="C31" t="s">
         <v>209</v>
       </c>
-      <c r="C30" t="s">
-        <v>66</v>
-      </c>
-      <c r="H30" t="s">
-        <v>52</v>
-      </c>
-      <c r="J30" s="5"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>44</v>
-      </c>
-      <c r="B31" t="s">
-        <v>45</v>
-      </c>
-      <c r="C31" t="s">
-        <v>46</v>
-      </c>
       <c r="D31" t="s">
-        <v>47</v>
-      </c>
-      <c r="G31" s="4" t="s">
-        <v>48</v>
+        <v>215</v>
+      </c>
+      <c r="E31" t="s">
+        <v>217</v>
+      </c>
+      <c r="F31" t="s">
+        <v>216</v>
       </c>
       <c r="H31" t="s">
-        <v>23</v>
-      </c>
-      <c r="I31" t="s">
-        <v>49</v>
+        <v>10</v>
+      </c>
+      <c r="I31" s="8" t="s">
+        <v>218</v>
       </c>
       <c r="J31" s="2"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>50</v>
+        <v>206</v>
       </c>
       <c r="C32" t="s">
-        <v>9</v>
+        <v>209</v>
       </c>
       <c r="D32" t="s">
-        <v>51</v>
+        <v>163</v>
       </c>
       <c r="E32" t="s">
-        <v>60</v>
+        <v>217</v>
       </c>
       <c r="F32" t="s">
-        <v>55</v>
-      </c>
-      <c r="G32" s="4" t="s">
-        <v>55</v>
+        <v>216</v>
       </c>
       <c r="H32" t="s">
-        <v>52</v>
-      </c>
-      <c r="I32" t="s">
-        <v>55</v>
-      </c>
-      <c r="J32" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="I32" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="J32" s="2"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>53</v>
+        <v>207</v>
       </c>
       <c r="C33" t="s">
-        <v>54</v>
-      </c>
-      <c r="D33" t="s">
-        <v>55</v>
-      </c>
-      <c r="E33" t="s">
-        <v>55</v>
-      </c>
-      <c r="F33" t="s">
-        <v>58</v>
-      </c>
-      <c r="G33" s="4" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="H33" t="s">
-        <v>10</v>
-      </c>
-      <c r="I33" t="s">
-        <v>57</v>
-      </c>
-      <c r="J33" s="2"/>
+        <v>52</v>
+      </c>
+      <c r="J33" s="5"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>70</v>
+        <v>208</v>
       </c>
       <c r="C34" t="s">
         <v>66</v>
       </c>
-      <c r="D34" t="s">
-        <v>72</v>
-      </c>
-      <c r="F34" t="s">
-        <v>55</v>
-      </c>
-      <c r="G34" s="4" t="s">
-        <v>55</v>
-      </c>
       <c r="H34" t="s">
         <v>52</v>
       </c>
-      <c r="I34" t="s">
-        <v>55</v>
-      </c>
       <c r="J34" s="5"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>44</v>
+      </c>
       <c r="B35" t="s">
-        <v>71</v>
+        <v>45</v>
       </c>
       <c r="C35" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="D35" t="s">
-        <v>73</v>
-      </c>
-      <c r="F35" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="H35" t="s">
-        <v>52</v>
+        <v>23</v>
       </c>
       <c r="I35" t="s">
-        <v>55</v>
-      </c>
-      <c r="J35" s="5"/>
+        <v>49</v>
+      </c>
+      <c r="J35" s="2"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>74</v>
-      </c>
       <c r="B36" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="C36" t="s">
-        <v>76</v>
+        <v>9</v>
       </c>
       <c r="D36" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E36" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="F36" t="s">
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>79</v>
+        <v>55</v>
       </c>
       <c r="H36" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="I36" t="s">
-        <v>78</v>
-      </c>
-      <c r="J36" s="2"/>
+        <v>55</v>
+      </c>
+      <c r="J36" s="5"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>81</v>
+        <v>53</v>
       </c>
       <c r="C37" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="D37" t="s">
-        <v>85</v>
+        <v>55</v>
+      </c>
+      <c r="E37" t="s">
+        <v>55</v>
       </c>
       <c r="F37" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H37" t="s">
-        <v>52</v>
-      </c>
-      <c r="J37" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="I37" t="s">
+        <v>57</v>
+      </c>
+      <c r="J37" s="2"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="C38" t="s">
         <v>66</v>
       </c>
       <c r="D38" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="F38" t="s">
         <v>55</v>
@@ -2088,21 +2107,21 @@
       </c>
       <c r="H38" t="s">
         <v>52</v>
+      </c>
+      <c r="I38" t="s">
+        <v>55</v>
       </c>
       <c r="J38" s="5"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="C39" t="s">
-        <v>9</v>
+        <v>66</v>
       </c>
       <c r="D39" t="s">
-        <v>87</v>
-      </c>
-      <c r="E39" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="F39" t="s">
         <v>55</v>
@@ -2113,110 +2132,110 @@
       <c r="H39" t="s">
         <v>52</v>
       </c>
+      <c r="I39" t="s">
+        <v>55</v>
+      </c>
       <c r="J39" s="5"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>74</v>
+      </c>
       <c r="B40" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="C40" t="s">
-        <v>9</v>
+        <v>76</v>
       </c>
       <c r="D40" t="s">
-        <v>88</v>
+        <v>55</v>
       </c>
       <c r="E40" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="F40" t="s">
-        <v>55</v>
+        <v>80</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="H40" t="s">
-        <v>52</v>
-      </c>
-      <c r="J40" s="5"/>
+        <v>23</v>
+      </c>
+      <c r="I40" t="s">
+        <v>78</v>
+      </c>
+      <c r="J40" s="2"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="C41" t="s">
-        <v>9</v>
+        <v>66</v>
       </c>
       <c r="D41" t="s">
-        <v>88</v>
-      </c>
-      <c r="E41" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="F41" t="s">
-        <v>98</v>
+        <v>55</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>55</v>
       </c>
       <c r="H41" t="s">
-        <v>10</v>
-      </c>
-      <c r="I41" t="s">
-        <v>97</v>
-      </c>
-      <c r="J41" s="2"/>
+        <v>52</v>
+      </c>
+      <c r="J41" s="5"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>89</v>
-      </c>
       <c r="B42" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C42" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="D42" t="s">
-        <v>55</v>
-      </c>
-      <c r="E42" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="F42" t="s">
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>79</v>
+        <v>55</v>
       </c>
       <c r="H42" t="s">
-        <v>23</v>
-      </c>
-      <c r="I42" t="s">
-        <v>78</v>
-      </c>
-      <c r="J42" s="2"/>
+        <v>52</v>
+      </c>
+      <c r="J42" s="5"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="C43" t="s">
-        <v>102</v>
+        <v>9</v>
       </c>
       <c r="D43" t="s">
-        <v>55</v>
+        <v>87</v>
       </c>
       <c r="E43" t="s">
-        <v>106</v>
+        <v>61</v>
+      </c>
+      <c r="F43" t="s">
+        <v>55</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>103</v>
+        <v>55</v>
       </c>
       <c r="H43" t="s">
         <v>52</v>
       </c>
-      <c r="J43" s="2"/>
+      <c r="J43" s="5"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="C44" t="s">
         <v>9</v>
@@ -2225,229 +2244,229 @@
         <v>88</v>
       </c>
       <c r="E44" t="s">
-        <v>92</v>
+        <v>61</v>
       </c>
       <c r="F44" t="s">
-        <v>98</v>
+        <v>55</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>55</v>
       </c>
       <c r="H44" t="s">
-        <v>10</v>
-      </c>
-      <c r="I44" t="s">
-        <v>97</v>
-      </c>
-      <c r="J44" s="2"/>
+        <v>52</v>
+      </c>
+      <c r="J44" s="5"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C45" t="s">
         <v>9</v>
       </c>
       <c r="D45" t="s">
-        <v>34</v>
+        <v>88</v>
       </c>
       <c r="E45" t="s">
         <v>92</v>
       </c>
       <c r="F45" t="s">
-        <v>14</v>
-      </c>
-      <c r="G45" s="4" t="s">
-        <v>15</v>
+        <v>98</v>
       </c>
       <c r="H45" t="s">
         <v>10</v>
       </c>
       <c r="I45" t="s">
-        <v>16</v>
+        <v>97</v>
       </c>
       <c r="J45" s="2"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>89</v>
+      </c>
       <c r="B46" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="C46" t="s">
-        <v>9</v>
+        <v>76</v>
       </c>
       <c r="D46" t="s">
-        <v>87</v>
+        <v>55</v>
       </c>
       <c r="E46" t="s">
-        <v>104</v>
+        <v>77</v>
       </c>
       <c r="F46" t="s">
-        <v>55</v>
+        <v>80</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="H46" t="s">
-        <v>52</v>
+        <v>23</v>
       </c>
       <c r="I46" t="s">
-        <v>55</v>
-      </c>
-      <c r="J46" s="5"/>
+        <v>78</v>
+      </c>
+      <c r="J46" s="2"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="C47" t="s">
-        <v>9</v>
+        <v>102</v>
       </c>
       <c r="D47" t="s">
-        <v>88</v>
+        <v>55</v>
       </c>
       <c r="E47" t="s">
-        <v>104</v>
-      </c>
-      <c r="F47" t="s">
-        <v>55</v>
+        <v>106</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>55</v>
+        <v>103</v>
       </c>
       <c r="H47" t="s">
         <v>52</v>
       </c>
-      <c r="J47" s="5"/>
+      <c r="J47" s="2"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C48" t="s">
-        <v>66</v>
+        <v>9</v>
       </c>
       <c r="D48" t="s">
-        <v>105</v>
+        <v>88</v>
+      </c>
+      <c r="E48" t="s">
+        <v>92</v>
       </c>
       <c r="F48" t="s">
-        <v>55</v>
-      </c>
-      <c r="G48" s="4" t="s">
-        <v>55</v>
+        <v>98</v>
       </c>
       <c r="H48" t="s">
-        <v>52</v>
+        <v>10</v>
       </c>
       <c r="I48" t="s">
-        <v>55</v>
-      </c>
-      <c r="J48" s="5"/>
+        <v>97</v>
+      </c>
+      <c r="J48" s="2"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C49" t="s">
-        <v>66</v>
+        <v>9</v>
       </c>
       <c r="D49" t="s">
-        <v>85</v>
+        <v>34</v>
+      </c>
+      <c r="E49" t="s">
+        <v>92</v>
       </c>
       <c r="F49" t="s">
-        <v>55</v>
+        <v>14</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="H49" t="s">
-        <v>52</v>
+        <v>10</v>
       </c>
       <c r="I49" t="s">
-        <v>55</v>
-      </c>
-      <c r="J49" s="5"/>
+        <v>16</v>
+      </c>
+      <c r="J49" s="2"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>112</v>
-      </c>
       <c r="B50" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="C50" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="D50" t="s">
-        <v>55</v>
+        <v>87</v>
       </c>
       <c r="E50" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="F50" t="s">
-        <v>110</v>
+        <v>55</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>111</v>
+        <v>55</v>
+      </c>
+      <c r="H50" t="s">
+        <v>52</v>
+      </c>
+      <c r="I50" t="s">
+        <v>55</v>
       </c>
       <c r="J50" s="5"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="C51" t="s">
-        <v>123</v>
+        <v>9</v>
       </c>
       <c r="D51" t="s">
-        <v>55</v>
+        <v>88</v>
       </c>
       <c r="E51" t="s">
-        <v>125</v>
+        <v>104</v>
       </c>
       <c r="F51" t="s">
-        <v>114</v>
-      </c>
-      <c r="G51" s="6" t="s">
-        <v>124</v>
+        <v>55</v>
+      </c>
+      <c r="G51" s="4" t="s">
+        <v>55</v>
       </c>
       <c r="H51" t="s">
-        <v>10</v>
-      </c>
-      <c r="I51" t="s">
-        <v>126</v>
+        <v>52</v>
       </c>
       <c r="J51" s="5"/>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>118</v>
+        <v>100</v>
       </c>
       <c r="C52" t="s">
-        <v>119</v>
-      </c>
-      <c r="E52" t="s">
-        <v>113</v>
+        <v>66</v>
+      </c>
+      <c r="D52" t="s">
+        <v>105</v>
       </c>
       <c r="F52" t="s">
-        <v>114</v>
-      </c>
-      <c r="G52" s="7" t="s">
-        <v>121</v>
+        <v>55</v>
+      </c>
+      <c r="G52" s="4" t="s">
+        <v>55</v>
       </c>
       <c r="H52" t="s">
-        <v>10</v>
+        <v>52</v>
       </c>
       <c r="I52" t="s">
-        <v>120</v>
+        <v>55</v>
       </c>
       <c r="J52" s="5"/>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>127</v>
+        <v>101</v>
       </c>
       <c r="C53" t="s">
-        <v>128</v>
-      </c>
-      <c r="E53" t="s">
-        <v>131</v>
+        <v>66</v>
+      </c>
+      <c r="D53" t="s">
+        <v>85</v>
       </c>
       <c r="F53" t="s">
         <v>55</v>
@@ -2464,431 +2483,479 @@
       <c r="J53" s="5"/>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>112</v>
+      </c>
       <c r="B54" t="s">
-        <v>129</v>
+        <v>108</v>
       </c>
       <c r="C54" t="s">
-        <v>128</v>
+        <v>54</v>
+      </c>
+      <c r="D54" t="s">
+        <v>55</v>
       </c>
       <c r="E54" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="F54" t="s">
-        <v>55</v>
+        <v>110</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>55</v>
+        <v>111</v>
       </c>
       <c r="H54" t="s">
-        <v>52</v>
-      </c>
-      <c r="I54" t="s">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="J54" s="5"/>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="C55" t="s">
-        <v>128</v>
+        <v>123</v>
+      </c>
+      <c r="D55" t="s">
+        <v>55</v>
       </c>
       <c r="E55" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="F55" t="s">
-        <v>55</v>
-      </c>
-      <c r="G55" s="4" t="s">
-        <v>55</v>
+        <v>114</v>
+      </c>
+      <c r="G55" s="6" t="s">
+        <v>124</v>
       </c>
       <c r="H55" t="s">
-        <v>52</v>
+        <v>10</v>
       </c>
       <c r="I55" t="s">
-        <v>55</v>
+        <v>126</v>
       </c>
       <c r="J55" s="5"/>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="C56" t="s">
-        <v>66</v>
-      </c>
-      <c r="D56" t="s">
-        <v>135</v>
+        <v>119</v>
+      </c>
+      <c r="E56" t="s">
+        <v>113</v>
       </c>
       <c r="F56" t="s">
-        <v>55</v>
-      </c>
-      <c r="G56" s="4" t="s">
-        <v>55</v>
+        <v>114</v>
+      </c>
+      <c r="G56" s="7" t="s">
+        <v>121</v>
       </c>
       <c r="H56" t="s">
-        <v>52</v>
+        <v>10</v>
       </c>
       <c r="I56" t="s">
-        <v>55</v>
+        <v>120</v>
       </c>
       <c r="J56" s="5"/>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="C57" t="s">
-        <v>66</v>
-      </c>
-      <c r="D57" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="E57" t="s">
-        <v>141</v>
-      </c>
-      <c r="J57" s="2"/>
+        <v>131</v>
+      </c>
+      <c r="F57" t="s">
+        <v>55</v>
+      </c>
+      <c r="G57" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H57" t="s">
+        <v>52</v>
+      </c>
+      <c r="I57" t="s">
+        <v>55</v>
+      </c>
+      <c r="J57" s="5"/>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="C58" t="s">
-        <v>66</v>
-      </c>
-      <c r="D58" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="E58" t="s">
-        <v>141</v>
-      </c>
-      <c r="J58" s="2"/>
+        <v>132</v>
+      </c>
+      <c r="F58" t="s">
+        <v>55</v>
+      </c>
+      <c r="G58" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H58" t="s">
+        <v>52</v>
+      </c>
+      <c r="I58" t="s">
+        <v>55</v>
+      </c>
+      <c r="J58" s="5"/>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="C59" t="s">
-        <v>66</v>
-      </c>
-      <c r="D59" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="E59" t="s">
-        <v>141</v>
-      </c>
-      <c r="J59" s="2"/>
+        <v>133</v>
+      </c>
+      <c r="F59" t="s">
+        <v>55</v>
+      </c>
+      <c r="G59" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H59" t="s">
+        <v>52</v>
+      </c>
+      <c r="I59" t="s">
+        <v>55</v>
+      </c>
+      <c r="J59" s="5"/>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C60" t="s">
         <v>66</v>
       </c>
       <c r="D60" t="s">
-        <v>140</v>
-      </c>
-      <c r="E60" t="s">
-        <v>141</v>
-      </c>
-      <c r="J60" s="2"/>
+        <v>135</v>
+      </c>
+      <c r="F60" t="s">
+        <v>55</v>
+      </c>
+      <c r="G60" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H60" t="s">
+        <v>52</v>
+      </c>
+      <c r="I60" t="s">
+        <v>55</v>
+      </c>
+      <c r="J60" s="5"/>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>211</v>
+        <v>136</v>
       </c>
       <c r="C61" t="s">
-        <v>102</v>
+        <v>66</v>
+      </c>
+      <c r="D61" t="s">
+        <v>140</v>
       </c>
       <c r="E61" t="s">
-        <v>212</v>
+        <v>141</v>
       </c>
       <c r="F61" t="s">
-        <v>213</v>
-      </c>
-      <c r="G61" s="4" t="s">
-        <v>214</v>
+        <v>239</v>
+      </c>
+      <c r="G61" s="13" t="s">
+        <v>240</v>
       </c>
       <c r="H61" t="s">
         <v>23</v>
       </c>
-      <c r="I61" s="9" t="s">
-        <v>215</v>
+      <c r="I61" t="s">
+        <v>241</v>
       </c>
       <c r="J61" s="2"/>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>142</v>
-      </c>
       <c r="B62" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="C62" t="s">
-        <v>9</v>
+        <v>66</v>
       </c>
       <c r="D62" t="s">
-        <v>161</v>
+        <v>140</v>
       </c>
       <c r="E62" t="s">
-        <v>104</v>
+        <v>141</v>
       </c>
       <c r="F62" t="s">
-        <v>55</v>
-      </c>
-      <c r="G62" s="4" t="s">
-        <v>55</v>
+        <v>239</v>
+      </c>
+      <c r="G62" s="13" t="s">
+        <v>240</v>
       </c>
       <c r="H62" t="s">
-        <v>52</v>
+        <v>23</v>
       </c>
       <c r="I62" t="s">
-        <v>55</v>
-      </c>
-      <c r="J62" s="5"/>
+        <v>241</v>
+      </c>
+      <c r="J62" s="2"/>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C63" t="s">
-        <v>9</v>
+        <v>66</v>
       </c>
       <c r="D63" t="s">
-        <v>162</v>
+        <v>140</v>
       </c>
       <c r="E63" t="s">
-        <v>104</v>
+        <v>141</v>
       </c>
       <c r="F63" t="s">
-        <v>55</v>
-      </c>
-      <c r="G63" s="4" t="s">
-        <v>55</v>
+        <v>239</v>
+      </c>
+      <c r="G63" s="13" t="s">
+        <v>240</v>
       </c>
       <c r="H63" t="s">
-        <v>52</v>
+        <v>23</v>
       </c>
       <c r="I63" t="s">
-        <v>55</v>
-      </c>
-      <c r="J63" s="5"/>
+        <v>241</v>
+      </c>
+      <c r="J63" s="2"/>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
+        <v>139</v>
+      </c>
+      <c r="C64" t="s">
+        <v>66</v>
+      </c>
+      <c r="D64" t="s">
+        <v>140</v>
+      </c>
+      <c r="E64" t="s">
+        <v>141</v>
+      </c>
+      <c r="F64" t="s">
+        <v>239</v>
+      </c>
+      <c r="G64" s="13" t="s">
+        <v>240</v>
+      </c>
+      <c r="H64" t="s">
+        <v>23</v>
+      </c>
+      <c r="I64" t="s">
+        <v>241</v>
+      </c>
+      <c r="J64" s="2"/>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>210</v>
+      </c>
+      <c r="C65" t="s">
+        <v>102</v>
+      </c>
+      <c r="E65" t="s">
+        <v>211</v>
+      </c>
+      <c r="F65" t="s">
+        <v>212</v>
+      </c>
+      <c r="G65" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="H65" t="s">
+        <v>23</v>
+      </c>
+      <c r="I65" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="J65" s="2"/>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>142</v>
+      </c>
+      <c r="B66" t="s">
+        <v>143</v>
+      </c>
+      <c r="C66" t="s">
+        <v>9</v>
+      </c>
+      <c r="D66" t="s">
+        <v>161</v>
+      </c>
+      <c r="E66" t="s">
+        <v>104</v>
+      </c>
+      <c r="F66" t="s">
+        <v>55</v>
+      </c>
+      <c r="G66" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H66" t="s">
+        <v>52</v>
+      </c>
+      <c r="I66" t="s">
+        <v>55</v>
+      </c>
+      <c r="J66" s="5"/>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>144</v>
+      </c>
+      <c r="C67" t="s">
+        <v>9</v>
+      </c>
+      <c r="D67" t="s">
+        <v>162</v>
+      </c>
+      <c r="E67" t="s">
+        <v>104</v>
+      </c>
+      <c r="F67" t="s">
+        <v>55</v>
+      </c>
+      <c r="G67" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H67" t="s">
+        <v>52</v>
+      </c>
+      <c r="I67" t="s">
+        <v>55</v>
+      </c>
+      <c r="J67" s="5"/>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
         <v>145</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C68" t="s">
         <v>9</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D68" t="s">
         <v>88</v>
       </c>
-      <c r="E64" t="s">
+      <c r="E68" t="s">
         <v>104</v>
       </c>
-      <c r="F64" t="s">
-        <v>55</v>
-      </c>
-      <c r="G64" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="H64" t="s">
-        <v>52</v>
-      </c>
-      <c r="I64" t="s">
-        <v>55</v>
-      </c>
-      <c r="J64" s="5"/>
-    </row>
-    <row r="65" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B65" t="s">
+      <c r="F68" t="s">
+        <v>55</v>
+      </c>
+      <c r="G68" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H68" t="s">
+        <v>52</v>
+      </c>
+      <c r="I68" t="s">
+        <v>55</v>
+      </c>
+      <c r="J68" s="5"/>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
         <v>146</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C69" t="s">
         <v>9</v>
       </c>
-      <c r="D65" t="s">
+      <c r="D69" t="s">
         <v>88</v>
       </c>
-      <c r="E65" t="s">
+      <c r="E69" t="s">
         <v>104</v>
       </c>
-      <c r="F65" t="s">
-        <v>55</v>
-      </c>
-      <c r="G65" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="H65" t="s">
-        <v>52</v>
-      </c>
-      <c r="I65" t="s">
-        <v>55</v>
-      </c>
-      <c r="J65" s="5"/>
-    </row>
-    <row r="66" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B66" t="s">
+      <c r="F69" t="s">
+        <v>55</v>
+      </c>
+      <c r="G69" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H69" t="s">
+        <v>52</v>
+      </c>
+      <c r="I69" t="s">
+        <v>55</v>
+      </c>
+      <c r="J69" s="5"/>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
         <v>147</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C70" t="s">
         <v>66</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D70" t="s">
         <v>165</v>
       </c>
-      <c r="F66" t="s">
-        <v>55</v>
-      </c>
-      <c r="G66" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="H66" t="s">
-        <v>52</v>
-      </c>
-      <c r="I66" t="s">
-        <v>55</v>
-      </c>
-      <c r="J66" s="5"/>
-    </row>
-    <row r="67" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B67" t="s">
+      <c r="F70" t="s">
+        <v>55</v>
+      </c>
+      <c r="G70" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H70" t="s">
+        <v>52</v>
+      </c>
+      <c r="I70" t="s">
+        <v>55</v>
+      </c>
+      <c r="J70" s="5"/>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
         <v>148</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C71" t="s">
         <v>66</v>
       </c>
-      <c r="D67" t="s">
+      <c r="D71" t="s">
         <v>163</v>
       </c>
-      <c r="F67" t="s">
-        <v>55</v>
-      </c>
-      <c r="G67" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="H67" t="s">
-        <v>52</v>
-      </c>
-      <c r="I67" t="s">
-        <v>55</v>
-      </c>
-      <c r="J67" s="5"/>
-    </row>
-    <row r="68" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B68" t="s">
+      <c r="F71" t="s">
+        <v>55</v>
+      </c>
+      <c r="G71" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H71" t="s">
+        <v>52</v>
+      </c>
+      <c r="I71" t="s">
+        <v>55</v>
+      </c>
+      <c r="J71" s="5"/>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
         <v>149</v>
-      </c>
-      <c r="C68" t="s">
-        <v>66</v>
-      </c>
-      <c r="D68" t="s">
-        <v>163</v>
-      </c>
-      <c r="F68" t="s">
-        <v>55</v>
-      </c>
-      <c r="G68" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="H68" t="s">
-        <v>52</v>
-      </c>
-      <c r="I68" t="s">
-        <v>55</v>
-      </c>
-      <c r="J68" s="5"/>
-    </row>
-    <row r="69" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B69" t="s">
-        <v>115</v>
-      </c>
-      <c r="C69" t="s">
-        <v>116</v>
-      </c>
-      <c r="D69" t="s">
-        <v>55</v>
-      </c>
-      <c r="E69" t="s">
-        <v>117</v>
-      </c>
-      <c r="F69" t="s">
-        <v>80</v>
-      </c>
-      <c r="G69" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="H69" t="s">
-        <v>10</v>
-      </c>
-      <c r="I69" t="s">
-        <v>152</v>
-      </c>
-      <c r="J69" s="5"/>
-    </row>
-    <row r="70" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B70" t="s">
-        <v>150</v>
-      </c>
-      <c r="C70" t="s">
-        <v>153</v>
-      </c>
-      <c r="D70" t="s">
-        <v>55</v>
-      </c>
-      <c r="E70" t="s">
-        <v>154</v>
-      </c>
-      <c r="F70" t="s">
-        <v>58</v>
-      </c>
-      <c r="G70" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="H70" t="s">
-        <v>10</v>
-      </c>
-      <c r="I70" t="s">
-        <v>155</v>
-      </c>
-      <c r="J70" s="5"/>
-    </row>
-    <row r="71" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B71" t="s">
-        <v>157</v>
-      </c>
-      <c r="C71" t="s">
-        <v>158</v>
-      </c>
-      <c r="D71" t="s">
-        <v>55</v>
-      </c>
-      <c r="F71" t="s">
-        <v>80</v>
-      </c>
-      <c r="G71" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="H71" t="s">
-        <v>10</v>
-      </c>
-      <c r="I71" t="s">
-        <v>160</v>
-      </c>
-      <c r="J71" s="5"/>
-    </row>
-    <row r="72" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B72" t="s">
-        <v>166</v>
       </c>
       <c r="C72" t="s">
         <v>66</v>
       </c>
       <c r="D72" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="F72" t="s">
         <v>55</v>
@@ -2904,90 +2971,93 @@
       </c>
       <c r="J72" s="5"/>
     </row>
-    <row r="73" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>167</v>
+        <v>115</v>
       </c>
       <c r="C73" t="s">
-        <v>66</v>
+        <v>116</v>
       </c>
       <c r="D73" t="s">
-        <v>173</v>
+        <v>55</v>
+      </c>
+      <c r="E73" t="s">
+        <v>117</v>
       </c>
       <c r="F73" t="s">
-        <v>55</v>
-      </c>
-      <c r="G73" s="4" t="s">
-        <v>55</v>
+        <v>80</v>
+      </c>
+      <c r="G73" s="6" t="s">
+        <v>151</v>
       </c>
       <c r="H73" t="s">
-        <v>52</v>
+        <v>10</v>
       </c>
       <c r="I73" t="s">
-        <v>55</v>
+        <v>152</v>
       </c>
       <c r="J73" s="5"/>
     </row>
-    <row r="74" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>168</v>
+        <v>150</v>
       </c>
       <c r="C74" t="s">
-        <v>66</v>
+        <v>153</v>
       </c>
       <c r="D74" t="s">
-        <v>164</v>
+        <v>55</v>
+      </c>
+      <c r="E74" t="s">
+        <v>154</v>
       </c>
       <c r="F74" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="G74" s="4" t="s">
-        <v>55</v>
+        <v>156</v>
       </c>
       <c r="H74" t="s">
-        <v>52</v>
+        <v>10</v>
       </c>
       <c r="I74" t="s">
-        <v>55</v>
+        <v>155</v>
       </c>
       <c r="J74" s="5"/>
     </row>
-    <row r="75" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="C75" t="s">
-        <v>66</v>
+        <v>158</v>
       </c>
       <c r="D75" t="s">
         <v>55</v>
       </c>
-      <c r="E75" t="s">
-        <v>174</v>
-      </c>
       <c r="F75" t="s">
-        <v>55</v>
-      </c>
-      <c r="G75" s="4" t="s">
-        <v>55</v>
+        <v>80</v>
+      </c>
+      <c r="G75" s="6" t="s">
+        <v>159</v>
       </c>
       <c r="H75" t="s">
-        <v>52</v>
+        <v>10</v>
       </c>
       <c r="I75" t="s">
-        <v>55</v>
+        <v>160</v>
       </c>
       <c r="J75" s="5"/>
     </row>
-    <row r="76" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C76" t="s">
         <v>66</v>
       </c>
       <c r="D76" t="s">
-        <v>163</v>
+        <v>172</v>
       </c>
       <c r="F76" t="s">
         <v>55</v>
@@ -3003,15 +3073,15 @@
       </c>
       <c r="J76" s="5"/>
     </row>
-    <row r="77" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C77" t="s">
         <v>66</v>
       </c>
       <c r="D77" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F77" t="s">
         <v>55</v>
@@ -3027,18 +3097,15 @@
       </c>
       <c r="J77" s="5"/>
     </row>
-    <row r="78" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="C78" t="s">
-        <v>9</v>
+        <v>66</v>
       </c>
       <c r="D78" t="s">
-        <v>182</v>
-      </c>
-      <c r="E78" t="s">
-        <v>184</v>
+        <v>164</v>
       </c>
       <c r="F78" t="s">
         <v>55</v>
@@ -3054,18 +3121,18 @@
       </c>
       <c r="J78" s="5"/>
     </row>
-    <row r="79" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="C79" t="s">
-        <v>9</v>
+        <v>66</v>
       </c>
       <c r="D79" t="s">
-        <v>88</v>
+        <v>55</v>
       </c>
       <c r="E79" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="F79" t="s">
         <v>55</v>
@@ -3081,18 +3148,15 @@
       </c>
       <c r="J79" s="5"/>
     </row>
-    <row r="80" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="C80" t="s">
-        <v>9</v>
+        <v>66</v>
       </c>
       <c r="D80" t="s">
-        <v>183</v>
-      </c>
-      <c r="E80" t="s">
-        <v>104</v>
+        <v>163</v>
       </c>
       <c r="F80" t="s">
         <v>55</v>
@@ -3110,16 +3174,13 @@
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="C81" t="s">
-        <v>9</v>
+        <v>66</v>
       </c>
       <c r="D81" t="s">
-        <v>88</v>
-      </c>
-      <c r="E81" t="s">
-        <v>104</v>
+        <v>172</v>
       </c>
       <c r="F81" t="s">
         <v>55</v>
@@ -3137,16 +3198,16 @@
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C82" t="s">
         <v>9</v>
       </c>
       <c r="D82" t="s">
-        <v>34</v>
+        <v>182</v>
       </c>
       <c r="E82" t="s">
-        <v>104</v>
+        <v>184</v>
       </c>
       <c r="F82" t="s">
         <v>55</v>
@@ -3164,147 +3225,182 @@
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C83" t="s">
-        <v>181</v>
+        <v>9</v>
+      </c>
+      <c r="D83" t="s">
+        <v>88</v>
       </c>
       <c r="E83" t="s">
-        <v>185</v>
-      </c>
-      <c r="J83" s="2"/>
+        <v>184</v>
+      </c>
+      <c r="F83" t="s">
+        <v>55</v>
+      </c>
+      <c r="G83" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H83" t="s">
+        <v>52</v>
+      </c>
+      <c r="I83" t="s">
+        <v>55</v>
+      </c>
+      <c r="J83" s="5"/>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>191</v>
-      </c>
+      <c r="B84" t="s">
+        <v>177</v>
+      </c>
+      <c r="C84" t="s">
+        <v>9</v>
+      </c>
+      <c r="D84" t="s">
+        <v>183</v>
+      </c>
+      <c r="E84" t="s">
+        <v>104</v>
+      </c>
+      <c r="F84" t="s">
+        <v>55</v>
+      </c>
+      <c r="G84" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H84" t="s">
+        <v>52</v>
+      </c>
+      <c r="I84" t="s">
+        <v>55</v>
+      </c>
+      <c r="J84" s="5"/>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
+        <v>178</v>
+      </c>
+      <c r="C85" t="s">
+        <v>9</v>
+      </c>
+      <c r="D85" t="s">
+        <v>88</v>
+      </c>
+      <c r="E85" t="s">
+        <v>104</v>
+      </c>
+      <c r="F85" t="s">
+        <v>55</v>
+      </c>
+      <c r="G85" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H85" t="s">
+        <v>52</v>
+      </c>
+      <c r="I85" t="s">
+        <v>55</v>
+      </c>
+      <c r="J85" s="5"/>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
+        <v>179</v>
+      </c>
+      <c r="C86" t="s">
+        <v>9</v>
+      </c>
+      <c r="D86" t="s">
+        <v>34</v>
+      </c>
+      <c r="E86" t="s">
+        <v>104</v>
+      </c>
+      <c r="F86" t="s">
+        <v>55</v>
+      </c>
+      <c r="G86" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H86" t="s">
+        <v>52</v>
+      </c>
+      <c r="I86" t="s">
+        <v>55</v>
+      </c>
+      <c r="J86" s="5"/>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>221</v>
+        <v>190</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C90" t="s">
+      <c r="K90" s="11"/>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B93" t="s">
+        <v>242</v>
+      </c>
+      <c r="C93" t="s">
+        <v>66</v>
+      </c>
+      <c r="D93" t="s">
+        <v>243</v>
+      </c>
+      <c r="E93" t="s">
+        <v>244</v>
+      </c>
+      <c r="F93" t="s">
+        <v>239</v>
+      </c>
+      <c r="G93" s="13" t="s">
+        <v>240</v>
+      </c>
+      <c r="H93" t="s">
+        <v>23</v>
+      </c>
+      <c r="I93" t="s">
+        <v>241</v>
+      </c>
+      <c r="J93" s="2"/>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B94" t="s">
+        <v>253</v>
+      </c>
+      <c r="C94" t="s">
+        <v>238</v>
+      </c>
+      <c r="F94" t="s">
+        <v>227</v>
+      </c>
+      <c r="G94" s="10" t="s">
         <v>228</v>
       </c>
-      <c r="F90" t="s">
+      <c r="H94" t="s">
+        <v>23</v>
+      </c>
+      <c r="I94" t="s">
         <v>229</v>
       </c>
-      <c r="G90" s="10" t="s">
-        <v>230</v>
-      </c>
-      <c r="H90" t="s">
-        <v>23</v>
-      </c>
-      <c r="I90" t="s">
-        <v>231</v>
-      </c>
-      <c r="J90" s="2"/>
-      <c r="K90" s="11"/>
-    </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C91" t="s">
-        <v>232</v>
-      </c>
-      <c r="E91" t="s">
-        <v>233</v>
-      </c>
-      <c r="F91" t="s">
-        <v>55</v>
-      </c>
-      <c r="G91" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="H91" t="s">
-        <v>52</v>
-      </c>
-      <c r="I91" t="s">
-        <v>55</v>
-      </c>
-      <c r="J91" s="5"/>
-    </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B92" t="s">
-        <v>236</v>
-      </c>
-      <c r="C92" t="s">
-        <v>210</v>
-      </c>
-      <c r="D92" t="s">
-        <v>237</v>
-      </c>
-      <c r="F92" t="s">
-        <v>217</v>
-      </c>
-      <c r="G92" t="s">
-        <v>239</v>
-      </c>
-      <c r="H92" t="s">
-        <v>10</v>
-      </c>
-      <c r="I92" t="s">
-        <v>238</v>
-      </c>
-      <c r="J92" s="2"/>
-    </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C93" t="s">
-        <v>234</v>
-      </c>
-      <c r="E93" t="s">
-        <v>235</v>
-      </c>
-      <c r="F93" t="s">
-        <v>55</v>
-      </c>
-      <c r="G93" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="H93" t="s">
-        <v>52</v>
-      </c>
-      <c r="I93" t="s">
-        <v>55</v>
-      </c>
-      <c r="J93" s="5"/>
-    </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>186</v>
-      </c>
-      <c r="B94" t="s">
-        <v>187</v>
-      </c>
-      <c r="C94" t="s">
-        <v>192</v>
-      </c>
-      <c r="E94" t="s">
-        <v>193</v>
-      </c>
-      <c r="F94" t="s">
-        <v>55</v>
-      </c>
-      <c r="G94" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="H94" t="s">
-        <v>52</v>
-      </c>
-      <c r="I94" t="s">
-        <v>55</v>
-      </c>
-      <c r="J94" s="5"/>
+      <c r="J94" s="2"/>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
-        <v>188</v>
+        <v>254</v>
       </c>
       <c r="C95" t="s">
-        <v>192</v>
+        <v>230</v>
       </c>
       <c r="E95" t="s">
-        <v>193</v>
+        <v>231</v>
       </c>
       <c r="F95" t="s">
         <v>55</v>
@@ -3322,78 +3418,312 @@
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
+        <v>234</v>
+      </c>
+      <c r="C96" t="s">
+        <v>209</v>
+      </c>
+      <c r="D96" t="s">
+        <v>235</v>
+      </c>
+      <c r="F96" t="s">
+        <v>216</v>
+      </c>
+      <c r="G96" t="s">
+        <v>237</v>
+      </c>
+      <c r="H96" t="s">
+        <v>10</v>
+      </c>
+      <c r="I96" t="s">
+        <v>236</v>
+      </c>
+      <c r="J96" s="2"/>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B97" t="s">
+        <v>252</v>
+      </c>
+      <c r="C97" t="s">
+        <v>232</v>
+      </c>
+      <c r="E97" t="s">
+        <v>233</v>
+      </c>
+      <c r="F97" t="s">
+        <v>55</v>
+      </c>
+      <c r="G97" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H97" t="s">
+        <v>52</v>
+      </c>
+      <c r="I97" t="s">
+        <v>55</v>
+      </c>
+      <c r="J97" s="5"/>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B98" t="s">
+        <v>248</v>
+      </c>
+      <c r="C98" t="s">
+        <v>9</v>
+      </c>
+      <c r="D98" s="14" t="s">
+        <v>256</v>
+      </c>
+      <c r="F98" t="s">
+        <v>55</v>
+      </c>
+      <c r="G98" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H98" t="s">
+        <v>52</v>
+      </c>
+      <c r="I98" t="s">
+        <v>55</v>
+      </c>
+      <c r="J98" s="5"/>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B99" t="s">
+        <v>249</v>
+      </c>
+      <c r="C99" t="s">
+        <v>9</v>
+      </c>
+      <c r="D99" t="s">
+        <v>88</v>
+      </c>
+      <c r="F99" t="s">
+        <v>55</v>
+      </c>
+      <c r="G99" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H99" t="s">
+        <v>52</v>
+      </c>
+      <c r="I99" t="s">
+        <v>55</v>
+      </c>
+      <c r="J99" s="5"/>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B100" t="s">
+        <v>250</v>
+      </c>
+      <c r="C100" t="s">
+        <v>66</v>
+      </c>
+      <c r="D100" t="s">
+        <v>257</v>
+      </c>
+      <c r="F100" t="s">
+        <v>55</v>
+      </c>
+      <c r="G100" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H100" t="s">
+        <v>52</v>
+      </c>
+      <c r="I100" t="s">
+        <v>55</v>
+      </c>
+      <c r="J100" s="5"/>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B101" t="s">
+        <v>251</v>
+      </c>
+      <c r="C101" t="s">
+        <v>66</v>
+      </c>
+      <c r="D101" t="s">
+        <v>258</v>
+      </c>
+      <c r="F101" t="s">
+        <v>55</v>
+      </c>
+      <c r="G101" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H101" t="s">
+        <v>52</v>
+      </c>
+      <c r="I101" t="s">
+        <v>55</v>
+      </c>
+      <c r="J101" s="5"/>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B102" t="s">
+        <v>255</v>
+      </c>
+      <c r="C102" t="s">
+        <v>66</v>
+      </c>
+      <c r="D102" t="s">
+        <v>259</v>
+      </c>
+      <c r="F102" t="s">
+        <v>55</v>
+      </c>
+      <c r="G102" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H102" t="s">
+        <v>52</v>
+      </c>
+      <c r="I102" t="s">
+        <v>55</v>
+      </c>
+      <c r="J102" s="5"/>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>185</v>
+      </c>
+      <c r="B103" t="s">
+        <v>186</v>
+      </c>
+      <c r="C103" t="s">
+        <v>191</v>
+      </c>
+      <c r="E103" t="s">
+        <v>192</v>
+      </c>
+      <c r="F103" t="s">
+        <v>55</v>
+      </c>
+      <c r="G103" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H103" t="s">
+        <v>52</v>
+      </c>
+      <c r="I103" t="s">
+        <v>55</v>
+      </c>
+      <c r="J103" s="5"/>
+      <c r="K103" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B104" t="s">
+        <v>187</v>
+      </c>
+      <c r="C104" t="s">
+        <v>191</v>
+      </c>
+      <c r="E104" t="s">
+        <v>192</v>
+      </c>
+      <c r="F104" t="s">
+        <v>55</v>
+      </c>
+      <c r="G104" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H104" t="s">
+        <v>52</v>
+      </c>
+      <c r="I104" t="s">
+        <v>55</v>
+      </c>
+      <c r="J104" s="5"/>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B105" t="s">
+        <v>188</v>
+      </c>
+      <c r="C105" t="s">
+        <v>191</v>
+      </c>
+      <c r="E105" t="s">
+        <v>192</v>
+      </c>
+      <c r="F105" t="s">
+        <v>55</v>
+      </c>
+      <c r="G105" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H105" t="s">
+        <v>52</v>
+      </c>
+      <c r="I105" t="s">
+        <v>55</v>
+      </c>
+      <c r="J105" s="5"/>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B106" t="s">
         <v>189</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C106" t="s">
+        <v>191</v>
+      </c>
+      <c r="E106" t="s">
         <v>192</v>
       </c>
-      <c r="E96" t="s">
-        <v>193</v>
-      </c>
-      <c r="F96" t="s">
-        <v>55</v>
-      </c>
-      <c r="G96" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="H96" t="s">
-        <v>52</v>
-      </c>
-      <c r="I96" t="s">
-        <v>55</v>
-      </c>
-      <c r="J96" s="5"/>
-    </row>
-    <row r="97" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B97" t="s">
-        <v>190</v>
-      </c>
-      <c r="C97" t="s">
-        <v>192</v>
-      </c>
-      <c r="E97" t="s">
-        <v>193</v>
-      </c>
-      <c r="F97" t="s">
-        <v>55</v>
-      </c>
-      <c r="G97" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="H97" t="s">
-        <v>52</v>
-      </c>
-      <c r="I97" t="s">
-        <v>55</v>
-      </c>
-      <c r="J97" s="5"/>
-    </row>
-    <row r="98" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B98" t="s">
+      <c r="F106" t="s">
+        <v>55</v>
+      </c>
+      <c r="G106" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H106" t="s">
+        <v>52</v>
+      </c>
+      <c r="I106" t="s">
+        <v>55</v>
+      </c>
+      <c r="J106" s="5"/>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B107" t="s">
+        <v>223</v>
+      </c>
+      <c r="C107" t="s">
+        <v>222</v>
+      </c>
+      <c r="D107" t="s">
+        <v>221</v>
+      </c>
+      <c r="E107" t="s">
+        <v>222</v>
+      </c>
+      <c r="G107" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="H107" t="s">
+        <v>10</v>
+      </c>
+      <c r="I107" t="s">
         <v>224</v>
       </c>
-      <c r="C98" t="s">
-        <v>223</v>
-      </c>
-      <c r="D98" t="s">
-        <v>222</v>
-      </c>
-      <c r="E98" t="s">
-        <v>223</v>
-      </c>
-      <c r="G98" s="4" t="s">
-        <v>226</v>
-      </c>
-      <c r="H98" t="s">
-        <v>10</v>
-      </c>
-      <c r="I98" t="s">
-        <v>225</v>
-      </c>
-      <c r="J98" s="2"/>
-      <c r="K98" t="s">
-        <v>227</v>
-      </c>
+      <c r="J107" s="2"/>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B108" t="s">
+        <v>180</v>
+      </c>
+      <c r="C108" t="s">
+        <v>181</v>
+      </c>
+      <c r="E108" t="s">
+        <v>245</v>
+      </c>
+      <c r="H108" t="s">
+        <v>52</v>
+      </c>
+      <c r="J108" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
recieved parts BOM update
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\max19_000\Documents\GitHub\Power2LabPowerSupply\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sjefen\OneDrive - Danmarks Tekniske Universitet\Skole\Effektelektronik 2\Power2LabPowerSupply\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9465"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9465" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="263">
   <si>
     <t>Circuit Block</t>
   </si>
@@ -807,12 +807,18 @@
   </si>
   <si>
     <t>545-2052</t>
+  </si>
+  <si>
+    <t>Received</t>
+  </si>
+  <si>
+    <t>10, but wrong part number</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1230,11 +1236,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K108"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L85" sqref="L85"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J114" sqref="J114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1251,7 +1257,7 @@
     <col min="10" max="10" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="27.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="27.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>12</v>
       </c>
@@ -1265,7 +1271,7 @@
       <c r="I1" s="14"/>
       <c r="J1" s="14"/>
     </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1296,8 +1302,11 @@
       <c r="J2" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1326,8 +1335,11 @@
         <v>16</v>
       </c>
       <c r="J3" s="5"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>17</v>
       </c>
@@ -1353,8 +1365,11 @@
         <v>16</v>
       </c>
       <c r="J4" s="5"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>18</v>
       </c>
@@ -1380,8 +1395,11 @@
         <v>16</v>
       </c>
       <c r="J5" s="5"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>21</v>
       </c>
@@ -1408,7 +1426,7 @@
       </c>
       <c r="J6" s="5"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>23</v>
       </c>
@@ -1435,7 +1453,7 @@
       </c>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>19</v>
       </c>
@@ -1462,7 +1480,7 @@
       </c>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>20</v>
       </c>
@@ -1489,7 +1507,7 @@
       </c>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>24</v>
       </c>
@@ -1516,7 +1534,7 @@
       </c>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>25</v>
       </c>
@@ -1536,8 +1554,11 @@
         <v>10</v>
       </c>
       <c r="J11" s="5"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>26</v>
       </c>
@@ -1557,8 +1578,11 @@
         <v>10</v>
       </c>
       <c r="J12" s="5"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>27</v>
       </c>
@@ -1582,7 +1606,7 @@
       </c>
       <c r="J13" s="5"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>28</v>
       </c>
@@ -1599,8 +1623,11 @@
         <v>49</v>
       </c>
       <c r="J14" s="5"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>29</v>
       </c>
@@ -1617,8 +1644,11 @@
         <v>49</v>
       </c>
       <c r="J15" s="5"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>30</v>
       </c>
@@ -1635,8 +1665,11 @@
         <v>49</v>
       </c>
       <c r="J16" s="5"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>60</v>
       </c>
@@ -1660,7 +1693,7 @@
       </c>
       <c r="J17" s="5"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>61</v>
       </c>
@@ -1684,7 +1717,7 @@
       </c>
       <c r="J18" s="5"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>62</v>
       </c>
@@ -1708,7 +1741,7 @@
       </c>
       <c r="J19" s="5"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>190</v>
       </c>
@@ -1737,8 +1770,11 @@
         <v>200</v>
       </c>
       <c r="J20" s="5"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K20">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>192</v>
       </c>
@@ -1764,8 +1800,11 @@
         <v>200</v>
       </c>
       <c r="J21" s="5"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K21" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>193</v>
       </c>
@@ -1791,8 +1830,11 @@
         <v>200</v>
       </c>
       <c r="J22" s="5"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K22" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>195</v>
       </c>
@@ -1818,8 +1860,11 @@
         <v>200</v>
       </c>
       <c r="J23" s="5"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K23" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>194</v>
       </c>
@@ -1845,8 +1890,11 @@
         <v>200</v>
       </c>
       <c r="J24" s="5"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K24" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>196</v>
       </c>
@@ -1872,8 +1920,11 @@
         <v>200</v>
       </c>
       <c r="J25" s="5"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K25" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>201</v>
       </c>
@@ -1891,7 +1942,7 @@
       </c>
       <c r="J26" s="5"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>239</v>
       </c>
@@ -1917,8 +1968,11 @@
         <v>200</v>
       </c>
       <c r="J27" s="5"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K27" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>240</v>
       </c>
@@ -1944,8 +1998,11 @@
         <v>200</v>
       </c>
       <c r="J28" s="5"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K28" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>202</v>
       </c>
@@ -1968,8 +2025,11 @@
         <v>212</v>
       </c>
       <c r="J31" s="5"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>203</v>
       </c>
@@ -1992,8 +2052,11 @@
         <v>213</v>
       </c>
       <c r="J32" s="5"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>204</v>
       </c>
@@ -2005,7 +2068,7 @@
       </c>
       <c r="J33" s="5"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>205</v>
       </c>
@@ -2017,7 +2080,7 @@
       </c>
       <c r="J34" s="5"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>41</v>
       </c>
@@ -2041,7 +2104,7 @@
       </c>
       <c r="J35" s="5"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>47</v>
       </c>
@@ -2068,7 +2131,7 @@
       </c>
       <c r="J36" s="5"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>50</v>
       </c>
@@ -2094,8 +2157,11 @@
         <v>54</v>
       </c>
       <c r="J37" s="5"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K37">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>67</v>
       </c>
@@ -2119,7 +2185,7 @@
       </c>
       <c r="J38" s="5"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>68</v>
       </c>
@@ -2143,7 +2209,7 @@
       </c>
       <c r="J39" s="5"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>71</v>
       </c>
@@ -2173,7 +2239,7 @@
       </c>
       <c r="J40" s="5"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>78</v>
       </c>
@@ -2194,7 +2260,7 @@
       </c>
       <c r="J41" s="5"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>79</v>
       </c>
@@ -2215,7 +2281,7 @@
       </c>
       <c r="J42" s="5"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>80</v>
       </c>
@@ -2239,7 +2305,7 @@
       </c>
       <c r="J43" s="5"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>81</v>
       </c>
@@ -2263,7 +2329,7 @@
       </c>
       <c r="J44" s="5"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>88</v>
       </c>
@@ -2286,8 +2352,11 @@
         <v>94</v>
       </c>
       <c r="J45" s="5"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K45" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>86</v>
       </c>
@@ -2317,7 +2386,7 @@
       </c>
       <c r="J46" s="5"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>91</v>
       </c>
@@ -2338,7 +2407,7 @@
       </c>
       <c r="J47" s="5"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>92</v>
       </c>
@@ -2361,8 +2430,11 @@
         <v>94</v>
       </c>
       <c r="J48" s="5"/>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K48" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>93</v>
       </c>
@@ -2388,8 +2460,11 @@
         <v>16</v>
       </c>
       <c r="J49" s="5"/>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K49" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>96</v>
       </c>
@@ -2416,7 +2491,7 @@
       </c>
       <c r="J50" s="5"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>104</v>
       </c>
@@ -2440,7 +2515,7 @@
       </c>
       <c r="J51" s="5"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>97</v>
       </c>
@@ -2464,7 +2539,7 @@
       </c>
       <c r="J52" s="5"/>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>98</v>
       </c>
@@ -2488,7 +2563,7 @@
       </c>
       <c r="J53" s="5"/>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>109</v>
       </c>
@@ -2514,8 +2589,11 @@
         <v>10</v>
       </c>
       <c r="J54" s="5"/>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K54">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>119</v>
       </c>
@@ -2542,7 +2620,7 @@
       </c>
       <c r="J55" s="5"/>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>115</v>
       </c>
@@ -2566,7 +2644,7 @@
       </c>
       <c r="J56" s="5"/>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>124</v>
       </c>
@@ -2590,7 +2668,7 @@
       </c>
       <c r="J57" s="5"/>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>126</v>
       </c>
@@ -2614,7 +2692,7 @@
       </c>
       <c r="J58" s="5"/>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>127</v>
       </c>
@@ -2638,7 +2716,7 @@
       </c>
       <c r="J59" s="5"/>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>131</v>
       </c>
@@ -2662,7 +2740,7 @@
       </c>
       <c r="J60" s="5"/>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>133</v>
       </c>
@@ -2689,7 +2767,7 @@
       </c>
       <c r="J61" s="5"/>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>134</v>
       </c>
@@ -2716,7 +2794,7 @@
       </c>
       <c r="J62" s="5"/>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
         <v>135</v>
       </c>
@@ -2743,7 +2821,7 @@
       </c>
       <c r="J63" s="5"/>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>136</v>
       </c>
@@ -2770,7 +2848,7 @@
       </c>
       <c r="J64" s="5"/>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>207</v>
       </c>
@@ -2793,8 +2871,11 @@
         <v>260</v>
       </c>
       <c r="J65" s="5"/>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K65">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>139</v>
       </c>
@@ -2824,7 +2905,7 @@
       </c>
       <c r="J66" s="5"/>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>141</v>
       </c>
@@ -2851,7 +2932,7 @@
       </c>
       <c r="J67" s="5"/>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>142</v>
       </c>
@@ -2878,7 +2959,7 @@
       </c>
       <c r="J68" s="5"/>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>143</v>
       </c>
@@ -2905,7 +2986,7 @@
       </c>
       <c r="J69" s="5"/>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
         <v>144</v>
       </c>
@@ -2929,7 +3010,7 @@
       </c>
       <c r="J70" s="5"/>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
         <v>145</v>
       </c>
@@ -2953,7 +3034,7 @@
       </c>
       <c r="J71" s="5"/>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
         <v>146</v>
       </c>
@@ -2977,7 +3058,7 @@
       </c>
       <c r="J72" s="5"/>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
         <v>112</v>
       </c>
@@ -3004,7 +3085,7 @@
       </c>
       <c r="J73" s="5"/>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
         <v>147</v>
       </c>
@@ -3031,7 +3112,7 @@
       </c>
       <c r="J74" s="5"/>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
         <v>154</v>
       </c>
@@ -3055,7 +3136,7 @@
       </c>
       <c r="J75" s="5"/>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
         <v>163</v>
       </c>
@@ -3079,7 +3160,7 @@
       </c>
       <c r="J76" s="5"/>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
         <v>164</v>
       </c>
@@ -3103,7 +3184,7 @@
       </c>
       <c r="J77" s="5"/>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
         <v>165</v>
       </c>
@@ -3127,7 +3208,7 @@
       </c>
       <c r="J78" s="5"/>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
         <v>166</v>
       </c>
@@ -3154,7 +3235,7 @@
       </c>
       <c r="J79" s="5"/>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
         <v>167</v>
       </c>
@@ -3445,6 +3526,9 @@
         <v>229</v>
       </c>
       <c r="J96" s="5"/>
+      <c r="K96">
+        <v>2</v>
+      </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B97" t="s">

</xml_diff>